<commit_message>
Corrección lista de Mitigación de Riesgos
Corrección y actualización de la lista de mitigación de riesgos
</commit_message>
<xml_diff>
--- a/Integradora/05_PuzzleTechnologies/Anexos/Herramienta para la Administración de Riesgos.xlsx
+++ b/Integradora/05_PuzzleTechnologies/Anexos/Herramienta para la Administración de Riesgos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dioxis\Desktop\Actividades de Integradora\Parcial2\Act05\Anexos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dioxis\Documents\GitHub\DistribuidoraMueblesMaravatio\Integradora\05_PuzzleTechnologies\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8430" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8430"/>
   </bookViews>
   <sheets>
     <sheet name="Identificacion" sheetId="9" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <definedName name="Print_Titles" localSheetId="1">'Detalle del Riesgo'!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="380">
   <si>
     <t>Contexto:</t>
   </si>
@@ -3527,6 +3528,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1393646</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>127966</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="581025" y="95250"/>
+          <a:ext cx="812621" cy="842341"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5961,7 +6011,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6293,8 +6343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="D16" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6306,9 +6356,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>127</v>
-      </c>
+      <c r="A3" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="160" t="s">
@@ -6514,9 +6562,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="167">
-        <v>1</v>
-      </c>
+      <c r="A31" s="167"/>
       <c r="B31" s="169"/>
       <c r="C31" s="163"/>
       <c r="D31" s="167" t="s">
@@ -6534,6 +6580,7 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6542,7 +6589,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AB783"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A334" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>